<commit_message>
updated source file. Fixed issue with zeros and VGGT7
</commit_message>
<xml_diff>
--- a/Simple_XLS_Importer/data/DP-MOD/Map_of_donors_Concluded_Final_funding.xlsx
+++ b/Simple_XLS_Importer/data/DP-MOD/Map_of_donors_Concluded_Final_funding.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlos\Documents\projects\landbook-importers\Simple_XLS_Importer\data\DP-MOD\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2355" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="1"/>
+    <workbookView xWindow="2352" yWindow="0" windowWidth="20736" windowHeight="11760" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
     <sheet name="metadata" sheetId="3" r:id="rId2"/>
     <sheet name="Metadata_Statistical_&amp;_Notes" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -411,9 +416,6 @@
   </si>
   <si>
     <t>Funding_concluded_Project</t>
-  </si>
-  <si>
-    <t>Total founding for concluded projects - 1'000 $</t>
   </si>
   <si>
     <r>
@@ -491,10 +493,6 @@
     <t>N of Non Missings</t>
   </si>
   <si>
-    <t>Total_Funding_Concluded_Project
-('000 $)</t>
-  </si>
-  <si>
     <t>org_acronym</t>
   </si>
   <si>
@@ -550,11 +548,17 @@
   <si>
     <t>MOD</t>
   </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Total founding for concluded projects -Current USD</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0000"/>
   </numFmts>
@@ -665,7 +669,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -677,15 +681,17 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -712,6 +718,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1036,1156 +1050,1249 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C112"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView showZeros="0" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="12.140625" style="12" customWidth="1"/>
-    <col min="3" max="3" width="34.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" style="11" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" style="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="30">
+    <row r="1" spans="1:3">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
-        <v>145</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>139</v>
+      <c r="B1" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="12" t="s">
-        <v>148</v>
+      <c r="B2" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C2" s="15">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C3">
-        <v>71.428573608398438</v>
+      <c r="B3" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C3" s="15">
+        <v>71428.573608398438</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="12" t="s">
-        <v>148</v>
+      <c r="B4" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C4" s="15">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="12" t="s">
-        <v>148</v>
+      <c r="B5" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C5" s="15">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C6">
-        <v>61.363636016845703</v>
+      <c r="B6" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C6" s="15">
+        <v>61363.636016845703</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C7">
-        <v>23000</v>
+      <c r="B7" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C7" s="15">
+        <v>23000000</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C8">
-        <v>23000</v>
+      <c r="B8" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C8" s="15">
+        <v>23000000</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C9">
-        <v>71.428573608398438</v>
+      <c r="B9" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C9" s="15">
+        <v>71428.573608398438</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="12" t="s">
-        <v>148</v>
+      <c r="B10" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C10" s="15">
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C11">
-        <v>525</v>
+      <c r="B11" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C11" s="15">
+        <v>525000</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C12">
-        <v>230.11363220214844</v>
+      <c r="B12" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C12" s="15">
+        <v>230113.63220214844</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="12" t="s">
-        <v>148</v>
+      <c r="B13" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C13" s="15">
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C14">
-        <v>253.24674987792969</v>
+      <c r="B14" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C14" s="15">
+        <v>253246.74987792969</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="12" t="s">
-        <v>148</v>
+      <c r="B15" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C15" s="15">
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="12" t="s">
-        <v>148</v>
+      <c r="B16" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C16" s="15">
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C17">
-        <v>3100</v>
+      <c r="B17" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C17" s="15">
+        <v>3100000</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C18">
-        <v>1120.26513671875</v>
+      <c r="B18" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C18" s="15">
+        <v>1120265.13671875</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="12" t="s">
-        <v>148</v>
+      <c r="B19" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C19" s="15">
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="12" t="s">
-        <v>148</v>
+      <c r="B20" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C20" s="15">
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C21">
-        <v>132.79220581054687</v>
+      <c r="B21" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C21" s="15">
+        <v>132792.20581054688</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C22">
-        <v>1541.6666259765625</v>
+      <c r="B22" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C22" s="15">
+        <v>1541666.6259765625</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="12" t="s">
-        <v>148</v>
+      <c r="B23" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C23" s="15">
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C24">
-        <v>181.81817626953125</v>
+      <c r="B24" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C24" s="15">
+        <v>181818.17626953125</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C25">
-        <v>1438.09521484375</v>
+      <c r="B25" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C25" s="15">
+        <v>1438095.21484375</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="12" t="s">
-        <v>148</v>
+      <c r="B26" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C26" s="15">
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C27">
-        <v>61.363636016845703</v>
+      <c r="B27" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C27" s="15">
+        <v>61363.636016845703</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C28">
-        <v>446.42855834960937</v>
+      <c r="B28" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C28" s="15">
+        <v>446428.55834960938</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C29">
-        <v>586.3636474609375</v>
+      <c r="B29" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C29" s="15">
+        <v>586363.6474609375</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C30">
-        <v>4668.75</v>
+      <c r="B30" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C30" s="15">
+        <v>4668750</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
         <v>30</v>
       </c>
-      <c r="B31" s="12" t="s">
-        <v>148</v>
+      <c r="B31" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C31" s="15">
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
         <v>31</v>
       </c>
-      <c r="B32" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C32">
-        <v>6140</v>
+      <c r="B32" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C32" s="15">
+        <v>6140000</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
         <v>32</v>
       </c>
-      <c r="B33" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C33">
-        <v>525</v>
+      <c r="B33" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C33" s="15">
+        <v>525000</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
         <v>33</v>
       </c>
-      <c r="B34" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C34">
-        <v>450</v>
+      <c r="B34" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C34" s="15">
+        <v>450000</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
         <v>34</v>
       </c>
-      <c r="B35" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C35">
-        <v>181.81817626953125</v>
+      <c r="B35" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C35" s="15">
+        <v>181818.17626953125</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
         <v>35</v>
       </c>
-      <c r="B36" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C36">
-        <v>525</v>
+      <c r="B36" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C36" s="15">
+        <v>525000</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
         <v>36</v>
       </c>
-      <c r="B37" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C37">
-        <v>4140</v>
+      <c r="B37" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C37" s="15">
+        <v>4140000</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
         <v>37</v>
       </c>
-      <c r="B38" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C38">
-        <v>6726.36376953125</v>
+      <c r="B38" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C38" s="15">
+        <v>6726363.76953125</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
         <v>38</v>
       </c>
-      <c r="B39" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C39">
-        <v>2540</v>
+      <c r="B39" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C39" s="15">
+        <v>2540000</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
         <v>39</v>
       </c>
-      <c r="B40" s="12" t="s">
-        <v>148</v>
+      <c r="B40" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C40" s="15">
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
         <v>40</v>
       </c>
-      <c r="B41" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C41">
-        <v>23000</v>
+      <c r="B41" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C41" s="15">
+        <v>23000000</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
         <v>41</v>
       </c>
-      <c r="B42" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C42">
-        <v>3986.363525390625</v>
+      <c r="B42" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C42" s="15">
+        <v>3986363.525390625</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
         <v>42</v>
       </c>
-      <c r="B43" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C43">
-        <v>1358.3333740234375</v>
+      <c r="B43" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C43" s="15">
+        <v>1358333.3740234375</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
         <v>43</v>
       </c>
-      <c r="B44" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C44">
-        <v>4500</v>
+      <c r="B44" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C44" s="15">
+        <v>4500000</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
         <v>44</v>
       </c>
-      <c r="B45" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C45">
-        <v>168.75</v>
+      <c r="B45" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C45" s="15">
+        <v>168750</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
         <v>45</v>
       </c>
-      <c r="B46" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C46">
-        <v>1733.3333740234375</v>
+      <c r="B46" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C46" s="15">
+        <v>1733333.3740234375</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
         <v>46</v>
       </c>
-      <c r="B47" s="12" t="s">
-        <v>148</v>
+      <c r="B47" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C47" s="15">
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
         <v>47</v>
       </c>
-      <c r="B48" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C48">
-        <v>525</v>
+      <c r="B48" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C48" s="15">
+        <v>525000</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
         <v>48</v>
       </c>
-      <c r="B49" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C49">
-        <v>764.61041259765625</v>
+      <c r="B49" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C49" s="15">
+        <v>764610.41259765625</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
         <v>49</v>
       </c>
-      <c r="B50" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C50">
-        <v>2450</v>
+      <c r="B50" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C50" s="15">
+        <v>2450000</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
         <v>50</v>
       </c>
-      <c r="B51" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C51">
-        <v>181.81817626953125</v>
+      <c r="B51" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C51" s="15">
+        <v>181818.17626953125</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
         <v>51</v>
       </c>
-      <c r="B52" s="12" t="s">
-        <v>148</v>
+      <c r="B52" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C52" s="15">
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
         <v>52</v>
       </c>
-      <c r="B53" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C53">
-        <v>181.81817626953125</v>
+      <c r="B53" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C53" s="15">
+        <v>181818.17626953125</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
         <v>53</v>
       </c>
-      <c r="B54" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C54">
-        <v>6586.4287109375</v>
+      <c r="B54" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C54" s="15">
+        <v>6586428.7109375</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
         <v>54</v>
       </c>
-      <c r="B55" s="12" t="s">
-        <v>148</v>
+      <c r="B55" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C55" s="15">
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
         <v>55</v>
       </c>
-      <c r="B56" s="12" t="s">
-        <v>148</v>
+      <c r="B56" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C56" s="15">
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
         <v>56</v>
       </c>
-      <c r="B57" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C57">
-        <v>925</v>
+      <c r="B57" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C57" s="15">
+        <v>925000</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
         <v>57</v>
       </c>
-      <c r="B58" s="12" t="s">
-        <v>148</v>
+      <c r="B58" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C58" s="15">
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
         <v>58</v>
       </c>
-      <c r="B59" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C59">
-        <v>4875</v>
+      <c r="B59" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C59" s="15">
+        <v>4875000</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
         <v>59</v>
       </c>
-      <c r="B60" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C60">
-        <v>132.79220581054687</v>
+      <c r="B60" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C60" s="15">
+        <v>132792.20581054688</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" t="s">
         <v>60</v>
       </c>
-      <c r="B61" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C61">
-        <v>821.4285888671875</v>
+      <c r="B61" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C61" s="15">
+        <v>821428.5888671875</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
         <v>61</v>
       </c>
-      <c r="B62" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C62">
-        <v>502.08334350585938</v>
+      <c r="B62" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C62" s="15">
+        <v>502083.34350585938</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
         <v>62</v>
       </c>
-      <c r="B63" s="12" t="s">
-        <v>148</v>
+      <c r="B63" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C63" s="15">
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
         <v>63</v>
       </c>
-      <c r="B64" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C64">
-        <v>333.33334350585937</v>
+      <c r="B64" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C64" s="15">
+        <v>333333.34350585938</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
         <v>64</v>
       </c>
-      <c r="B65" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C65">
-        <v>2266.666748046875</v>
+      <c r="B65" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C65" s="15">
+        <v>2266666.748046875</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="s">
         <v>65</v>
       </c>
-      <c r="B66" s="12" t="s">
-        <v>148</v>
+      <c r="B66" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C66" s="15">
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" t="s">
         <v>66</v>
       </c>
-      <c r="B67" s="12" t="s">
-        <v>148</v>
+      <c r="B67" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C67" s="15">
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" t="s">
         <v>67</v>
       </c>
-      <c r="B68" s="12" t="s">
-        <v>148</v>
+      <c r="B68" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C68" s="15">
+        <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
         <v>68</v>
       </c>
-      <c r="B69" s="12" t="s">
-        <v>148</v>
+      <c r="B69" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C69" s="15">
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
         <v>69</v>
       </c>
-      <c r="B70" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C70">
-        <v>1186.3636474609375</v>
+      <c r="B70" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C70" s="15">
+        <v>1186363.6474609375</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" t="s">
         <v>70</v>
       </c>
-      <c r="B71" s="12" t="s">
-        <v>148</v>
+      <c r="B71" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C71" s="15">
+        <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72" t="s">
         <v>71</v>
       </c>
-      <c r="B72" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C72">
-        <v>1154.761962890625</v>
+      <c r="B72" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C72" s="15">
+        <v>1154761.962890625</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" t="s">
         <v>72</v>
       </c>
-      <c r="B73" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C73">
-        <v>61.363636016845703</v>
+      <c r="B73" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C73" s="15">
+        <v>61363.636016845703</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" t="s">
         <v>73</v>
       </c>
-      <c r="B74" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C74">
-        <v>525</v>
+      <c r="B74" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C74" s="15">
+        <v>525000</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" t="s">
         <v>74</v>
       </c>
-      <c r="B75" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C75">
-        <v>230.11363220214844</v>
+      <c r="B75" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C75" s="15">
+        <v>230113.63220214844</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" t="s">
         <v>75</v>
       </c>
-      <c r="B76" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C76">
-        <v>436.3636474609375</v>
+      <c r="B76" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C76" s="15">
+        <v>436363.6474609375</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" t="s">
         <v>76</v>
       </c>
-      <c r="B77" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C77">
-        <v>181.81817626953125</v>
+      <c r="B77" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C77" s="15">
+        <v>181818.17626953125</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" t="s">
         <v>77</v>
       </c>
-      <c r="B78" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C78">
-        <v>525</v>
+      <c r="B78" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C78" s="15">
+        <v>525000</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="s">
         <v>78</v>
       </c>
-      <c r="B79" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C79">
-        <v>1800</v>
+      <c r="B79" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C79" s="15">
+        <v>1800000</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
         <v>79</v>
       </c>
-      <c r="B80" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C80">
-        <v>2338.09521484375</v>
+      <c r="B80" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C80" s="15">
+        <v>2338095.21484375</v>
       </c>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" t="s">
         <v>80</v>
       </c>
-      <c r="B81" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C81">
-        <v>71.428573608398438</v>
+      <c r="B81" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C81" s="15">
+        <v>71428.573608398438</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" t="s">
         <v>81</v>
       </c>
-      <c r="B82" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C82">
-        <v>61.363636016845703</v>
+      <c r="B82" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C82" s="15">
+        <v>61363.636016845703</v>
       </c>
     </row>
     <row r="83" spans="1:3">
       <c r="A83" t="s">
         <v>82</v>
       </c>
-      <c r="B83" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C83">
-        <v>61.363636016845703</v>
+      <c r="B83" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C83" s="15">
+        <v>61363.636016845703</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" t="s">
         <v>83</v>
       </c>
-      <c r="B84" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C84">
-        <v>740</v>
+      <c r="B84" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C84" s="15">
+        <v>740000</v>
       </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" t="s">
         <v>84</v>
       </c>
-      <c r="B85" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C85">
-        <v>938.44696044921875</v>
+      <c r="B85" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C85" s="15">
+        <v>938446.96044921875</v>
       </c>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" t="s">
         <v>85</v>
       </c>
-      <c r="B86" s="12" t="s">
-        <v>148</v>
+      <c r="B86" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C86" s="15">
+        <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:3">
       <c r="A87" t="s">
         <v>86</v>
       </c>
-      <c r="B87" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C87">
-        <v>4500</v>
+      <c r="B87" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C87" s="15">
+        <v>4500000</v>
       </c>
     </row>
     <row r="88" spans="1:3">
       <c r="A88" t="s">
         <v>87</v>
       </c>
-      <c r="B88" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C88">
-        <v>2540</v>
+      <c r="B88" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C88" s="15">
+        <v>2540000</v>
       </c>
     </row>
     <row r="89" spans="1:3">
       <c r="A89" t="s">
         <v>88</v>
       </c>
-      <c r="B89" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C89">
-        <v>2000</v>
+      <c r="B89" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C89" s="15">
+        <v>2000000</v>
       </c>
     </row>
     <row r="90" spans="1:3">
       <c r="A90" t="s">
         <v>89</v>
       </c>
-      <c r="B90" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C90">
-        <v>1125</v>
+      <c r="B90" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C90" s="15">
+        <v>1125000</v>
       </c>
     </row>
     <row r="91" spans="1:3">
       <c r="A91" t="s">
         <v>90</v>
       </c>
-      <c r="B91" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C91">
-        <v>7040</v>
+      <c r="B91" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C91" s="15">
+        <v>7040000</v>
       </c>
     </row>
     <row r="92" spans="1:3">
       <c r="A92" t="s">
         <v>91</v>
       </c>
-      <c r="B92" s="12" t="s">
-        <v>148</v>
+      <c r="B92" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C92" s="15">
+        <v>0</v>
       </c>
     </row>
     <row r="93" spans="1:3">
       <c r="A93" t="s">
         <v>92</v>
       </c>
-      <c r="B93" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C93">
-        <v>6140</v>
+      <c r="B93" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C93" s="15">
+        <v>6140000</v>
       </c>
     </row>
     <row r="94" spans="1:3">
       <c r="A94" t="s">
         <v>93</v>
       </c>
-      <c r="B94" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C94">
-        <v>1733.3333740234375</v>
+      <c r="B94" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C94" s="15">
+        <v>1733333.3740234375</v>
       </c>
     </row>
     <row r="95" spans="1:3">
       <c r="A95" t="s">
         <v>94</v>
       </c>
-      <c r="B95" s="12" t="s">
-        <v>148</v>
+      <c r="B95" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C95" s="15">
+        <v>0</v>
       </c>
     </row>
     <row r="96" spans="1:3">
       <c r="A96" t="s">
         <v>95</v>
       </c>
-      <c r="B96" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C96">
-        <v>181.81817626953125</v>
+      <c r="B96" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C96" s="15">
+        <v>181818.17626953125</v>
       </c>
     </row>
     <row r="97" spans="1:3">
       <c r="A97" t="s">
         <v>96</v>
       </c>
-      <c r="B97" s="12" t="s">
-        <v>148</v>
+      <c r="B97" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C97" s="15">
+        <v>0</v>
       </c>
     </row>
     <row r="98" spans="1:3">
       <c r="A98" t="s">
         <v>97</v>
       </c>
-      <c r="B98" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C98">
-        <v>375</v>
+      <c r="B98" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C98" s="15">
+        <v>375000</v>
       </c>
     </row>
     <row r="99" spans="1:3">
       <c r="A99" t="s">
         <v>98</v>
       </c>
-      <c r="B99" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C99">
-        <v>250</v>
+      <c r="B99" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C99" s="15">
+        <v>250000</v>
       </c>
     </row>
     <row r="100" spans="1:3">
       <c r="A100" t="s">
         <v>99</v>
       </c>
-      <c r="B100" s="12" t="s">
-        <v>148</v>
+      <c r="B100" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C100" s="15">
+        <v>0</v>
       </c>
     </row>
     <row r="101" spans="1:3">
       <c r="A101" t="s">
         <v>100</v>
       </c>
-      <c r="B101" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C101">
-        <v>573.51190185546875</v>
+      <c r="B101" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C101" s="15">
+        <v>573511.90185546875</v>
       </c>
     </row>
     <row r="102" spans="1:3">
       <c r="A102" t="s">
         <v>101</v>
       </c>
-      <c r="B102" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C102">
-        <v>740</v>
+      <c r="B102" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C102" s="15">
+        <v>740000</v>
       </c>
     </row>
     <row r="103" spans="1:3">
       <c r="A103" t="s">
         <v>102</v>
       </c>
-      <c r="B103" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C103">
-        <v>181.81817626953125</v>
+      <c r="B103" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C103" s="15">
+        <v>181818.17626953125</v>
       </c>
     </row>
     <row r="104" spans="1:3">
       <c r="A104" t="s">
         <v>103</v>
       </c>
-      <c r="B104" s="12" t="s">
-        <v>148</v>
+      <c r="B104" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C104" s="15">
+        <v>0</v>
       </c>
     </row>
     <row r="105" spans="1:3">
       <c r="A105" t="s">
         <v>104</v>
       </c>
-      <c r="B105" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C105">
-        <v>894.69696044921875</v>
+      <c r="B105" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C105" s="15">
+        <v>894696.96044921875</v>
       </c>
     </row>
     <row r="106" spans="1:3">
       <c r="A106" t="s">
         <v>105</v>
       </c>
-      <c r="B106" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C106">
-        <v>61.363636016845703</v>
+      <c r="B106" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C106" s="15">
+        <v>61363.636016845703</v>
       </c>
     </row>
     <row r="107" spans="1:3">
       <c r="A107" t="s">
         <v>106</v>
       </c>
-      <c r="B107" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C107">
-        <v>181.81817626953125</v>
+      <c r="B107" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C107" s="15">
+        <v>181818.17626953125</v>
       </c>
     </row>
     <row r="108" spans="1:3">
       <c r="A108" t="s">
         <v>107</v>
       </c>
-      <c r="B108" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C108">
-        <v>2540</v>
+      <c r="B108" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C108" s="15">
+        <v>2540000</v>
       </c>
     </row>
     <row r="109" spans="1:3">
       <c r="A109" t="s">
         <v>108</v>
       </c>
-      <c r="B109" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C109">
-        <v>1236.3636474609375</v>
+      <c r="B109" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C109" s="15">
+        <v>1236363.6474609375</v>
       </c>
     </row>
     <row r="110" spans="1:3">
       <c r="A110" t="s">
         <v>109</v>
       </c>
-      <c r="B110" s="12" t="s">
-        <v>148</v>
+      <c r="B110" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C110" s="15">
+        <v>0</v>
       </c>
     </row>
     <row r="111" spans="1:3">
       <c r="A111" t="s">
         <v>110</v>
       </c>
-      <c r="B111" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C111">
-        <v>811.3636474609375</v>
+      <c r="B111" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C111" s="15">
+        <v>811363.6474609375</v>
       </c>
     </row>
     <row r="112" spans="1:3">
       <c r="A112" t="s">
         <v>111</v>
       </c>
-      <c r="B112" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C112">
-        <v>811.3636474609375</v>
+      <c r="B112" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C112" s="15">
+        <v>811363.6474609375</v>
       </c>
     </row>
   </sheetData>
@@ -2200,48 +2307,48 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="B1" s="13" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="10" t="s">
+      <c r="B3" s="12" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="B2" s="13" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>142</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="10" t="s">
-        <v>143</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -2250,70 +2357,70 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="14.1" customHeight="1">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="16" t="s">
         <v>118</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="I1" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="J1" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="K1" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="J1" s="14" t="s">
-        <v>120</v>
-      </c>
-      <c r="K1" s="16" t="s">
-        <v>138</v>
-      </c>
-      <c r="L1" s="14" t="s">
+      <c r="L1" s="16" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" s="15"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="15"/>
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="17"/>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="2" t="s">
@@ -2409,8 +2516,8 @@
       <c r="A6" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>130</v>
+      <c r="B6" s="13" t="s">
+        <v>151</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>128</v>
@@ -2445,7 +2552,7 @@
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -2458,7 +2565,7 @@
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="6" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -2473,7 +2580,7 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="6" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -2487,7 +2594,7 @@
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -2502,7 +2609,7 @@
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -2517,7 +2624,7 @@
     </row>
     <row r="14" spans="1:12">
       <c r="A14" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -2532,7 +2639,7 @@
     </row>
     <row r="15" spans="1:12">
       <c r="A15" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -2544,7 +2651,7 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>

</xml_diff>